<commit_message>
added variables for power level and class to raw data.
</commit_message>
<xml_diff>
--- a/data/raw_data/exampledata.xlsx
+++ b/data/raw_data/exampledata.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20348"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59FA2285-62C7-443A-BFBC-77E0754551CF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBF36E5C-5D8E-4E91-866F-652485BF93D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="11">
   <si>
     <t>Height</t>
   </si>
@@ -29,6 +29,30 @@
   </si>
   <si>
     <t>sixty</t>
+  </si>
+  <si>
+    <t>Power Level</t>
+  </si>
+  <si>
+    <t>&gt; 9000</t>
+  </si>
+  <si>
+    <t>Class</t>
+  </si>
+  <si>
+    <t>Wizard</t>
+  </si>
+  <si>
+    <t>Thief</t>
+  </si>
+  <si>
+    <t>Warrior</t>
+  </si>
+  <si>
+    <t>Fighter</t>
+  </si>
+  <si>
+    <t>Bard</t>
   </si>
 </sst>
 </file>
@@ -346,129 +370,219 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>180</v>
       </c>
       <c r="B2">
         <v>80</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C2">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>175</v>
       </c>
       <c r="B3">
         <v>70</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C3">
+        <v>11000</v>
+      </c>
+      <c r="D3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4">
         <v>60</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C4">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>178</v>
       </c>
       <c r="B5">
         <v>76</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C5">
+        <v>3</v>
+      </c>
+      <c r="D5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>192</v>
       </c>
       <c r="B6">
         <v>90</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C6">
+        <v>4.2</v>
+      </c>
+      <c r="D6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7">
         <v>55</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C7">
+        <v>150</v>
+      </c>
+      <c r="D7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>156</v>
       </c>
       <c r="B8">
         <v>90</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C8">
+        <v>150</v>
+      </c>
+      <c r="D8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>166</v>
       </c>
       <c r="B9">
         <v>110</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C9">
+        <v>210</v>
+      </c>
+      <c r="D9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>155</v>
       </c>
       <c r="B10">
         <v>54</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C10">
+        <v>1450</v>
+      </c>
+      <c r="D10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>145</v>
       </c>
       <c r="B11">
         <v>7000</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C11">
+        <v>710</v>
+      </c>
+      <c r="D11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>165</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C12">
+        <v>6</v>
+      </c>
+      <c r="D12" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>133</v>
       </c>
       <c r="B13">
         <v>45</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>166</v>
       </c>
       <c r="B14">
         <v>55</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C14">
+        <v>12</v>
+      </c>
+      <c r="D14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>154</v>
       </c>
       <c r="B15">
         <v>50</v>
+      </c>
+      <c r="C15">
+        <v>0.01</v>
+      </c>
+      <c r="D15" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix: fixed file name to match directions
</commit_message>
<xml_diff>
--- a/data/raw_data/exampledata.xlsx
+++ b/data/raw_data/exampledata.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20348"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBF36E5C-5D8E-4E91-866F-652485BF93D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59FA2285-62C7-443A-BFBC-77E0754551CF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>Height</t>
   </si>
@@ -29,30 +29,6 @@
   </si>
   <si>
     <t>sixty</t>
-  </si>
-  <si>
-    <t>Power Level</t>
-  </si>
-  <si>
-    <t>&gt; 9000</t>
-  </si>
-  <si>
-    <t>Class</t>
-  </si>
-  <si>
-    <t>Wizard</t>
-  </si>
-  <si>
-    <t>Thief</t>
-  </si>
-  <si>
-    <t>Warrior</t>
-  </si>
-  <si>
-    <t>Fighter</t>
-  </si>
-  <si>
-    <t>Bard</t>
   </si>
 </sst>
 </file>
@@ -370,219 +346,129 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>180</v>
       </c>
       <c r="B2">
         <v>80</v>
       </c>
-      <c r="C2">
-        <v>2</v>
-      </c>
-      <c r="D2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>175</v>
       </c>
       <c r="B3">
         <v>70</v>
       </c>
-      <c r="C3">
-        <v>11000</v>
-      </c>
-      <c r="D3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4">
         <v>60</v>
       </c>
-      <c r="C4">
-        <v>10</v>
-      </c>
-      <c r="D4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>178</v>
       </c>
       <c r="B5">
         <v>76</v>
       </c>
-      <c r="C5">
-        <v>3</v>
-      </c>
-      <c r="D5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>192</v>
       </c>
       <c r="B6">
         <v>90</v>
       </c>
-      <c r="C6">
-        <v>4.2</v>
-      </c>
-      <c r="D6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7">
         <v>55</v>
       </c>
-      <c r="C7">
-        <v>150</v>
-      </c>
-      <c r="D7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>156</v>
       </c>
       <c r="B8">
         <v>90</v>
       </c>
-      <c r="C8">
-        <v>150</v>
-      </c>
-      <c r="D8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A9">
         <v>166</v>
       </c>
       <c r="B9">
         <v>110</v>
       </c>
-      <c r="C9">
-        <v>210</v>
-      </c>
-      <c r="D9" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A10">
         <v>155</v>
       </c>
       <c r="B10">
         <v>54</v>
       </c>
-      <c r="C10">
-        <v>1450</v>
-      </c>
-      <c r="D10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A11">
         <v>145</v>
       </c>
       <c r="B11">
         <v>7000</v>
       </c>
-      <c r="C11">
-        <v>710</v>
-      </c>
-      <c r="D11" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A12">
         <v>165</v>
       </c>
-      <c r="C12">
-        <v>6</v>
-      </c>
-      <c r="D12" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A13">
         <v>133</v>
       </c>
       <c r="B13">
         <v>45</v>
       </c>
-      <c r="C13" t="s">
-        <v>4</v>
-      </c>
-      <c r="D13" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A14">
         <v>166</v>
       </c>
       <c r="B14">
         <v>55</v>
       </c>
-      <c r="C14">
-        <v>12</v>
-      </c>
-      <c r="D14" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A15">
         <v>154</v>
       </c>
       <c r="B15">
         <v>50</v>
-      </c>
-      <c r="C15">
-        <v>0.01</v>
-      </c>
-      <c r="D15" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>